<commit_message>
Filter spaces from Nutrient name and add a couple of nutrients for Soya Milk.
</commit_message>
<xml_diff>
--- a/Files/InsertyStatementsForFoodFromWaitroseNutrition.xlsx
+++ b/Files/InsertyStatementsForFoodFromWaitroseNutrition.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\HealthDb\HealthDb\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32897B94-C98F-4B28-8AB9-76A75DE5E7DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E78C3C8-6EBB-4FF2-857A-838AEA38A766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{BDD3D9AA-30AD-4471-9985-58E79E43B90A}"/>
   </bookViews>
   <sheets>
     <sheet name="T-SQL" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
   <si>
     <t>Typical values</t>
   </si>
@@ -81,9 +82,6 @@
     <t>Fibre</t>
   </si>
   <si>
-    <t>0.6g</t>
-  </si>
-  <si>
     <t>Protein</t>
   </si>
   <si>
@@ -108,43 +106,115 @@
     <t>Past Values from Waitrose Below</t>
   </si>
   <si>
-    <t>100g contains</t>
-  </si>
-  <si>
-    <t>78kJ</t>
-  </si>
-  <si>
-    <t>19kcal</t>
-  </si>
-  <si>
-    <t>0.1g</t>
-  </si>
-  <si>
     <t>0.0g</t>
   </si>
   <si>
-    <t>1.0g</t>
-  </si>
-  <si>
-    <t>2.6g</t>
-  </si>
-  <si>
     <t>0.08g</t>
   </si>
   <si>
-    <t>0.5g</t>
-  </si>
-  <si>
-    <t>Waitrose Essential Spinach</t>
-  </si>
-  <si>
     <t>DB Name</t>
   </si>
   <si>
-    <t>Essential Spinach</t>
-  </si>
-  <si>
     <t>Don't need this</t>
+  </si>
+  <si>
+    <t>PER 100ml</t>
+  </si>
+  <si>
+    <t>PER 250ml SERVING</t>
+  </si>
+  <si>
+    <t>146kJ</t>
+  </si>
+  <si>
+    <t>364kJ</t>
+  </si>
+  <si>
+    <t>35kcal</t>
+  </si>
+  <si>
+    <t>87kcal</t>
+  </si>
+  <si>
+    <t>1.9g</t>
+  </si>
+  <si>
+    <t>4.8g</t>
+  </si>
+  <si>
+    <t>0.3g</t>
+  </si>
+  <si>
+    <t>0.8g</t>
+  </si>
+  <si>
+    <t>2.0g</t>
+  </si>
+  <si>
+    <t>&lt;0.5g</t>
+  </si>
+  <si>
+    <t>1.2g</t>
+  </si>
+  <si>
+    <t>3.4g</t>
+  </si>
+  <si>
+    <t>8.5g</t>
+  </si>
+  <si>
+    <t>0.03g</t>
+  </si>
+  <si>
+    <t>Vitamin D</t>
+  </si>
+  <si>
+    <t>0.75µg</t>
+  </si>
+  <si>
+    <t>1.9µg</t>
+  </si>
+  <si>
+    <t>Riboflavin</t>
+  </si>
+  <si>
+    <t>0.21mg</t>
+  </si>
+  <si>
+    <t>0.53mg</t>
+  </si>
+  <si>
+    <t>Vitamin B12</t>
+  </si>
+  <si>
+    <t>0.38µg</t>
+  </si>
+  <si>
+    <t>0.95µg</t>
+  </si>
+  <si>
+    <t>Calcium</t>
+  </si>
+  <si>
+    <t>120mg</t>
+  </si>
+  <si>
+    <t>300mg</t>
+  </si>
+  <si>
+    <t>Iodine</t>
+  </si>
+  <si>
+    <t>22.4µg</t>
+  </si>
+  <si>
+    <t>56.0µg</t>
+  </si>
+  <si>
+    <t>Essential Soya Unsweetened Milk Alternative</t>
+  </si>
+  <si>
+    <t>Waitrose Essential Soya Drink Unsweetened</t>
   </si>
 </sst>
 </file>
@@ -190,10 +260,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -534,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E46BB2D-F735-4A55-BC5F-E1B4375D9E84}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -552,11 +621,11 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="72">
-      <c r="A1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="3" t="str">
+    <row r="1" spans="1:8" ht="72">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="str">
         <f>"DECLARE @FoodId INT
 DECLARE @kj NVARCHAR(20)='kj'
 DECLARE @g NVARCHAR(20)='g'
@@ -570,39 +639,39 @@
 DECLARE @ml NVARCHAR(20)='ml'
 DECLARE @µg NVARCHAR(20)='µg'</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="str">
         <f>"INSERT dbo.Foods (Name, Description) VALUES ('"&amp;A2&amp;"', '"&amp;B2&amp;"')"</f>
-        <v>INSERT dbo.Foods (Name, Description) VALUES ('Waitrose Essential Spinach', 'Essential Spinach')</v>
+        <v>INSERT dbo.Foods (Name, Description) VALUES ('Waitrose Essential Soya Drink Unsweetened', 'Essential Soya Unsweetened Milk Alternative')</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -610,7 +679,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(A5,"of which saturates","FatSaturates"),"of which sugars","CarbohydrateSugar")</f>
@@ -633,7 +702,7 @@
         <v>100</v>
       </c>
       <c r="F5" s="1" t="str" cm="1">
-        <f t="array" ref="F5">_xlfn.TEXTJOIN(
+        <f t="array" ref="F5">SUBSTITUTE(_xlfn.TEXTJOIN(
   "",
   ,
   IF(
@@ -644,12 +713,12 @@
     MID(B5,_xlfn.SEQUENCE(LEN(B5)),1),
     ""
   )
-)</f>
-        <v>gcontains</v>
+),"&lt;","")</f>
+        <v>PERml</v>
       </c>
       <c r="G5" s="1" t="str">
-        <f>TRIM(SUBSTITUTE(SUBSTITUTE(F5,"per",""),"contains",""))</f>
-        <v>g</v>
+        <f>TRIM(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(F5,"per",""),"contains",""),"PER",""))</f>
+        <v>ml</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -657,15 +726,15 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="str">
-        <f t="shared" ref="C6:C14" si="0">SUBSTITUTE(SUBSTITUTE(A6,"of which saturates","FatSaturates"),"of which sugars","CarbohydrateSugar")</f>
+        <f t="shared" ref="C6:C19" si="0">SUBSTITUTE(SUBSTITUTE(A6,"of which saturates","FatSaturates"),"of which sugars","CarbohydrateSugar")</f>
         <v>Energy</v>
       </c>
       <c r="D6" s="1" t="str">
         <f>IF(F6&lt;&gt;"kcal","(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = '"&amp;C6&amp;"' AND Unit='"&amp;F6&amp;"'), "&amp;E6&amp;", '"&amp;G$5&amp;"', "&amp;E$5&amp;"),","")</f>
-        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'Energy' AND Unit='kJ'), 78, 'g', 100),</v>
+        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'Energy' AND Unit='kJ'), 146, 'ml', 100),</v>
       </c>
       <c r="E6" s="1" cm="1">
         <f t="array" ref="E6">VALUE(
@@ -681,10 +750,10 @@
     )
   )
 )</f>
-        <v>78</v>
+        <v>146</v>
       </c>
       <c r="F6" s="1" t="str" cm="1">
-        <f t="array" ref="F6">_xlfn.TEXTJOIN(
+        <f t="array" ref="F6">SUBSTITUTE(_xlfn.TEXTJOIN(
   "",
   ,
   IF(
@@ -695,7 +764,7 @@
     MID(B6,_xlfn.SEQUENCE(LEN(B6)),1),
     ""
   )
-)</f>
+),"&lt;","")</f>
         <v>kJ</v>
       </c>
     </row>
@@ -704,7 +773,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -728,10 +797,10 @@
     )
   )
 )</f>
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="F7" s="1" t="str" cm="1">
-        <f t="array" ref="F7">_xlfn.TEXTJOIN(
+        <f t="array" ref="F7">SUBSTITUTE(_xlfn.TEXTJOIN(
   "",
   ,
   IF(
@@ -742,11 +811,11 @@
     MID(B7,_xlfn.SEQUENCE(LEN(B7)),1),
     ""
   )
-)</f>
+),"&lt;","")</f>
         <v>kcal</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -754,15 +823,15 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A8,"of which saturates","FatSaturates"),"of which sugars","CarbohydrateSugar")," ","")</f>
         <v>Fat</v>
       </c>
       <c r="D8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'Fat' AND Unit='g'), 0.6, 'g', 100),</v>
+        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'Fat' AND Unit='g'), 1.9, 'ml', 100),</v>
       </c>
       <c r="E8" s="1" cm="1">
         <f t="array" ref="E8">VALUE(
@@ -778,10 +847,10 @@
     )
   )
 )</f>
-        <v>0.6</v>
+        <v>1.9</v>
       </c>
       <c r="F8" s="1" t="str" cm="1">
-        <f t="array" ref="F8">_xlfn.TEXTJOIN(
+        <f t="array" ref="F8">SUBSTITUTE(_xlfn.TEXTJOIN(
   "",
   ,
   IF(
@@ -792,7 +861,7 @@
     MID(B8,_xlfn.SEQUENCE(LEN(B8)),1),
     ""
   )
-)</f>
+),"&lt;","")</f>
         <v>g</v>
       </c>
     </row>
@@ -801,15 +870,15 @@
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C9:C19" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(A9,"of which saturates","FatSaturates"),"of which sugars","CarbohydrateSugar")," ","")</f>
         <v>FatSaturates</v>
       </c>
       <c r="D9" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'FatSaturates' AND Unit='g'), 0.1, 'g', 100),</v>
+        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'FatSaturates' AND Unit='g'), 0.3, 'ml', 100),</v>
       </c>
       <c r="E9" s="1" cm="1">
         <f t="array" ref="E9">VALUE(
@@ -825,10 +894,10 @@
     )
   )
 )</f>
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="F9" s="1" t="str" cm="1">
-        <f t="array" ref="F9">_xlfn.TEXTJOIN(
+        <f t="array" ref="F9">SUBSTITUTE(_xlfn.TEXTJOIN(
   "",
   ,
   IF(
@@ -839,7 +908,7 @@
     MID(B9,_xlfn.SEQUENCE(LEN(B9)),1),
     ""
   )
-)</f>
+),"&lt;","")</f>
         <v>g</v>
       </c>
     </row>
@@ -848,15 +917,15 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C10" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Carbohydrate</v>
       </c>
       <c r="D10" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'Carbohydrate' AND Unit='g'), 0.5, 'g', 100),</v>
+        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'Carbohydrate' AND Unit='g'), 0.8, 'ml', 100),</v>
       </c>
       <c r="E10" s="1" cm="1">
         <f t="array" ref="E10">VALUE(
@@ -872,10 +941,10 @@
     )
   )
 )</f>
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="F10" s="1" t="str" cm="1">
-        <f t="array" ref="F10">_xlfn.TEXTJOIN(
+        <f t="array" ref="F10">SUBSTITUTE(_xlfn.TEXTJOIN(
   "",
   ,
   IF(
@@ -886,7 +955,7 @@
     MID(B10,_xlfn.SEQUENCE(LEN(B10)),1),
     ""
   )
-)</f>
+),"&lt;","")</f>
         <v>g</v>
       </c>
     </row>
@@ -895,15 +964,15 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>CarbohydrateSugar</v>
       </c>
       <c r="D11" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'CarbohydrateSugar' AND Unit='g'), 0, 'g', 100),</v>
+        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'CarbohydrateSugar' AND Unit='g'), 0, 'ml', 100),</v>
       </c>
       <c r="E11" s="1" cm="1">
         <f t="array" ref="E11">VALUE(
@@ -922,7 +991,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="1" t="str" cm="1">
-        <f t="array" ref="F11">_xlfn.TEXTJOIN(
+        <f t="array" ref="F11">SUBSTITUTE(_xlfn.TEXTJOIN(
   "",
   ,
   IF(
@@ -933,7 +1002,7 @@
     MID(B11,_xlfn.SEQUENCE(LEN(B11)),1),
     ""
   )
-)</f>
+),"&lt;","")</f>
         <v>g</v>
       </c>
     </row>
@@ -942,15 +1011,15 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Fibre</v>
       </c>
       <c r="D12" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'Fibre' AND Unit='g'), 1, 'g', 100),</v>
+        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'Fibre' AND Unit='g'), 0.5, 'ml', 100),</v>
       </c>
       <c r="E12" s="1" cm="1">
         <f t="array" ref="E12">VALUE(
@@ -966,10 +1035,10 @@
     )
   )
 )</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F12" s="1" t="str" cm="1">
-        <f t="array" ref="F12">_xlfn.TEXTJOIN(
+        <f t="array" ref="F12">SUBSTITUTE(_xlfn.TEXTJOIN(
   "",
   ,
   IF(
@@ -980,24 +1049,24 @@
     MID(B12,_xlfn.SEQUENCE(LEN(B12)),1),
     ""
   )
-)</f>
+),"&lt;","")</f>
         <v>g</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C13" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Protein</v>
       </c>
       <c r="D13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'Protein' AND Unit='g'), 2.6, 'g', 100),</v>
+        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'Protein' AND Unit='g'), 3.4, 'ml', 100),</v>
       </c>
       <c r="E13" s="1" cm="1">
         <f t="array" ref="E13">VALUE(
@@ -1013,10 +1082,10 @@
     )
   )
 )</f>
-        <v>2.6</v>
+        <v>3.4</v>
       </c>
       <c r="F13" s="1" t="str" cm="1">
-        <f t="array" ref="F13">_xlfn.TEXTJOIN(
+        <f t="array" ref="F13">SUBSTITUTE(_xlfn.TEXTJOIN(
   "",
   ,
   IF(
@@ -1027,24 +1096,24 @@
     MID(B13,_xlfn.SEQUENCE(LEN(B13)),1),
     ""
   )
-)</f>
+),"&lt;","")</f>
         <v>g</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C14" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Salt</v>
       </c>
       <c r="D14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'Salt' AND Unit='g'), 0.08, 'g', 100),</v>
+        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'Salt' AND Unit='g'), 0.03, 'ml', 100),</v>
       </c>
       <c r="E14" s="1" cm="1">
         <f t="array" ref="E14">VALUE(
@@ -1060,10 +1129,10 @@
     )
   )
 )</f>
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
       <c r="F14" s="1" t="str" cm="1">
-        <f t="array" ref="F14">_xlfn.TEXTJOIN(
+        <f t="array" ref="F14">SUBSTITUTE(_xlfn.TEXTJOIN(
   "",
   ,
   IF(
@@ -1074,8 +1143,428 @@
     MID(B14,_xlfn.SEQUENCE(LEN(B14)),1),
     ""
   )
+),"&lt;","")</f>
+        <v>g</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>VitaminD</v>
+      </c>
+      <c r="D15" s="1" t="str">
+        <f t="shared" ref="D15:D20" si="3">IF(F15&lt;&gt;"kcal","(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = '"&amp;C15&amp;"' AND Unit='"&amp;F15&amp;"'), "&amp;E15&amp;", '"&amp;G$5&amp;"', "&amp;E$5&amp;"),","")</f>
+        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'VitaminD' AND Unit='µg'), 0.75, 'ml', 100),</v>
+      </c>
+      <c r="E15" s="1" cm="1">
+        <f t="array" ref="E15">VALUE(
+  _xlfn.TEXTJOIN(
+    "",
+    ,
+    IF(
+      (ISNUMBER(--MID(B15,_xlfn.SEQUENCE(LEN(B15)),1)))
+        + (MID(B15,_xlfn.SEQUENCE(LEN(B15)),1)=".")
+        + (MID(B15,_xlfn.SEQUENCE(LEN(B15)),1)=",") &gt; 0,
+      MID(B15,_xlfn.SEQUENCE(LEN(B15)),1),
+      ""
+    )
+  )
 )</f>
-        <v>g</v>
+        <v>0.75</v>
+      </c>
+      <c r="F15" s="1" t="str" cm="1">
+        <f t="array" ref="F15">SUBSTITUTE(_xlfn.TEXTJOIN(
+  "",
+  ,
+  IF(
+    NOT(ISNUMBER(--MID(B15,_xlfn.SEQUENCE(LEN(B15)),1)))
+      * (MID(B15,_xlfn.SEQUENCE(LEN(B15)),1)&lt;&gt;",")
+      * (MID(B15,_xlfn.SEQUENCE(LEN(B15)),1)&lt;&gt;".")
+      * (MID(B15,_xlfn.SEQUENCE(LEN(B15)),1)&lt;&gt;" "),
+    MID(B15,_xlfn.SEQUENCE(LEN(B15)),1),
+    ""
+  )
+),"&lt;","")</f>
+        <v>µg</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Riboflavin</v>
+      </c>
+      <c r="D16" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'Riboflavin' AND Unit='mg'), 0.21, 'ml', 100),</v>
+      </c>
+      <c r="E16" s="1" cm="1">
+        <f t="array" ref="E16">VALUE(
+  _xlfn.TEXTJOIN(
+    "",
+    ,
+    IF(
+      (ISNUMBER(--MID(B16,_xlfn.SEQUENCE(LEN(B16)),1)))
+        + (MID(B16,_xlfn.SEQUENCE(LEN(B16)),1)=".")
+        + (MID(B16,_xlfn.SEQUENCE(LEN(B16)),1)=",") &gt; 0,
+      MID(B16,_xlfn.SEQUENCE(LEN(B16)),1),
+      ""
+    )
+  )
+)</f>
+        <v>0.21</v>
+      </c>
+      <c r="F16" s="1" t="str" cm="1">
+        <f t="array" ref="F16">SUBSTITUTE(_xlfn.TEXTJOIN(
+  "",
+  ,
+  IF(
+    NOT(ISNUMBER(--MID(B16,_xlfn.SEQUENCE(LEN(B16)),1)))
+      * (MID(B16,_xlfn.SEQUENCE(LEN(B16)),1)&lt;&gt;",")
+      * (MID(B16,_xlfn.SEQUENCE(LEN(B16)),1)&lt;&gt;".")
+      * (MID(B16,_xlfn.SEQUENCE(LEN(B16)),1)&lt;&gt;" "),
+    MID(B16,_xlfn.SEQUENCE(LEN(B16)),1),
+    ""
+  )
+),"&lt;","")</f>
+        <v>mg</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>VitaminB12</v>
+      </c>
+      <c r="D17" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'VitaminB12' AND Unit='µg'), 0.38, 'ml', 100),</v>
+      </c>
+      <c r="E17" s="1" cm="1">
+        <f t="array" ref="E17">VALUE(
+  _xlfn.TEXTJOIN(
+    "",
+    ,
+    IF(
+      (ISNUMBER(--MID(B17,_xlfn.SEQUENCE(LEN(B17)),1)))
+        + (MID(B17,_xlfn.SEQUENCE(LEN(B17)),1)=".")
+        + (MID(B17,_xlfn.SEQUENCE(LEN(B17)),1)=",") &gt; 0,
+      MID(B17,_xlfn.SEQUENCE(LEN(B17)),1),
+      ""
+    )
+  )
+)</f>
+        <v>0.38</v>
+      </c>
+      <c r="F17" s="1" t="str" cm="1">
+        <f t="array" ref="F17">SUBSTITUTE(_xlfn.TEXTJOIN(
+  "",
+  ,
+  IF(
+    NOT(ISNUMBER(--MID(B17,_xlfn.SEQUENCE(LEN(B17)),1)))
+      * (MID(B17,_xlfn.SEQUENCE(LEN(B17)),1)&lt;&gt;",")
+      * (MID(B17,_xlfn.SEQUENCE(LEN(B17)),1)&lt;&gt;".")
+      * (MID(B17,_xlfn.SEQUENCE(LEN(B17)),1)&lt;&gt;" "),
+    MID(B17,_xlfn.SEQUENCE(LEN(B17)),1),
+    ""
+  )
+),"&lt;","")</f>
+        <v>µg</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Calcium</v>
+      </c>
+      <c r="D18" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'Calcium' AND Unit='mg'), 120, 'ml', 100),</v>
+      </c>
+      <c r="E18" s="1" cm="1">
+        <f t="array" ref="E18">VALUE(
+  _xlfn.TEXTJOIN(
+    "",
+    ,
+    IF(
+      (ISNUMBER(--MID(B18,_xlfn.SEQUENCE(LEN(B18)),1)))
+        + (MID(B18,_xlfn.SEQUENCE(LEN(B18)),1)=".")
+        + (MID(B18,_xlfn.SEQUENCE(LEN(B18)),1)=",") &gt; 0,
+      MID(B18,_xlfn.SEQUENCE(LEN(B18)),1),
+      ""
+    )
+  )
+)</f>
+        <v>120</v>
+      </c>
+      <c r="F18" s="1" t="str" cm="1">
+        <f t="array" ref="F18">SUBSTITUTE(_xlfn.TEXTJOIN(
+  "",
+  ,
+  IF(
+    NOT(ISNUMBER(--MID(B18,_xlfn.SEQUENCE(LEN(B18)),1)))
+      * (MID(B18,_xlfn.SEQUENCE(LEN(B18)),1)&lt;&gt;",")
+      * (MID(B18,_xlfn.SEQUENCE(LEN(B18)),1)&lt;&gt;".")
+      * (MID(B18,_xlfn.SEQUENCE(LEN(B18)),1)&lt;&gt;" "),
+    MID(B18,_xlfn.SEQUENCE(LEN(B18)),1),
+    ""
+  )
+),"&lt;","")</f>
+        <v>mg</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Iodine</v>
+      </c>
+      <c r="D19" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>(@FoodId, (SELECT Id FROM dbo.Nutrients WHERE Name = 'Iodine' AND Unit='µg'), 22.4, 'ml', 100),</v>
+      </c>
+      <c r="E19" s="1" cm="1">
+        <f t="array" ref="E19">VALUE(
+  _xlfn.TEXTJOIN(
+    "",
+    ,
+    IF(
+      (ISNUMBER(--MID(B19,_xlfn.SEQUENCE(LEN(B19)),1)))
+        + (MID(B19,_xlfn.SEQUENCE(LEN(B19)),1)=".")
+        + (MID(B19,_xlfn.SEQUENCE(LEN(B19)),1)=",") &gt; 0,
+      MID(B19,_xlfn.SEQUENCE(LEN(B19)),1),
+      ""
+    )
+  )
+)</f>
+        <v>22.4</v>
+      </c>
+      <c r="F19" s="1" t="str" cm="1">
+        <f t="array" ref="F19">SUBSTITUTE(_xlfn.TEXTJOIN(
+  "",
+  ,
+  IF(
+    NOT(ISNUMBER(--MID(B19,_xlfn.SEQUENCE(LEN(B19)),1)))
+      * (MID(B19,_xlfn.SEQUENCE(LEN(B19)),1)&lt;&gt;",")
+      * (MID(B19,_xlfn.SEQUENCE(LEN(B19)),1)&lt;&gt;".")
+      * (MID(B19,_xlfn.SEQUENCE(LEN(B19)),1)&lt;&gt;" "),
+    MID(B19,_xlfn.SEQUENCE(LEN(B19)),1),
+    ""
+  )
+),"&lt;","")</f>
+        <v>µg</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B88866D-D5E4-451D-8B1A-9B40AF864FFA}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>